<commit_message>
RPS stuff as well as elec water units fix and pass-through fixes for refined liquids.  Note that refined liquids needs more work.
</commit_message>
<xml_diff>
--- a/rgcam-data-system/rgcam-data/Assumptions/Tables_RefLiq_Data.xlsx
+++ b/rgcam-data-system/rgcam-data/Assumptions/Tables_RefLiq_Data.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2000" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="2000" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Legend" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="93">
   <si>
     <t>This workbook collects refinery assumptions from the refined liquids workbook and reorganizes it into tables readily usable in the R procoessing</t>
   </si>
@@ -305,6 +305,12 @@
   <si>
     <t>PrimaryFuelCO2Coef</t>
   </si>
+  <si>
+    <t>marginal_rev_sector</t>
+  </si>
+  <si>
+    <t>marginal_rev_market</t>
+  </si>
 </sst>
 </file>
 
@@ -404,8 +410,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="599">
+  <cellStyleXfs count="605">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1019,7 +1031,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="599">
+  <cellStyles count="605">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1319,6 +1331,9 @@
     <cellStyle name="Followed Hyperlink" xfId="594" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="596" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="598" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="600" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="602" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="604" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1618,6 +1633,9 @@
     <cellStyle name="Hyperlink" xfId="593" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="595" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="597" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="599" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="601" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="603" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -7287,7 +7305,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
@@ -9381,30 +9399,30 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:8">
       <c r="A3" s="7" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -9423,8 +9441,14 @@
       <c r="F4" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4" t="s">
+        <v>91</v>
+      </c>
+      <c r="H4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="str">
         <f>Legend!A5</f>
         <v>oil refined liquids</v>
@@ -9447,8 +9471,15 @@
       <c r="F5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5" t="str">
+        <f>Legend!$A$9</f>
+        <v>refined liquids</v>
+      </c>
+      <c r="H5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="str">
         <f>Legend!A6</f>
         <v>biomass refined liquids</v>
@@ -9471,8 +9502,15 @@
       <c r="F6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6" t="str">
+        <f>Legend!$A$9</f>
+        <v>refined liquids</v>
+      </c>
+      <c r="H6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="str">
         <f>Legend!A7</f>
         <v>gas refined liquids</v>
@@ -9495,8 +9533,15 @@
       <c r="F7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7" t="str">
+        <f>Legend!$A$9</f>
+        <v>refined liquids</v>
+      </c>
+      <c r="H7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" t="str">
         <f>Legend!A8</f>
         <v>coal refined liquids</v>
@@ -9519,8 +9564,15 @@
       <c r="F8" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8" t="str">
+        <f>Legend!$A$9</f>
+        <v>refined liquids</v>
+      </c>
+      <c r="H8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" t="str">
         <f>Legend!A9</f>
         <v>refined liquids</v>
@@ -9545,7 +9597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:8">
       <c r="A10" t="str">
         <f>Legend!A10</f>
         <v>refined liquids enduse</v>
@@ -9569,7 +9621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:8">
       <c r="A11" t="str">
         <f>Legend!A11</f>
         <v>refined liquids industrial</v>
@@ -9595,6 +9647,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -9607,7 +9660,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>

</xml_diff>